<commit_message>
added product categories in FE
</commit_message>
<xml_diff>
--- a/files/documentation/Frontend Functionalities.xlsx
+++ b/files/documentation/Frontend Functionalities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1189EFD3-AAE0-42EF-BBDB-10C5E3CA58C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E058D3FF-E7E9-4374-B1DF-282BCF07D14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
made great progress with add product page
</commit_message>
<xml_diff>
--- a/files/documentation/Frontend Functionalities.xlsx
+++ b/files/documentation/Frontend Functionalities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E058D3FF-E7E9-4374-B1DF-282BCF07D14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EE9746-2807-42FC-9A5E-41C95A0940AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Functionality</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>User update username</t>
+  </si>
+  <si>
+    <t>Update Product</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,6 +688,15 @@
       </c>
       <c r="C24" s="2"/>
     </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished product add functionality
</commit_message>
<xml_diff>
--- a/files/documentation/Frontend Functionalities.xlsx
+++ b/files/documentation/Frontend Functionalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EE9746-2807-42FC-9A5E-41C95A0940AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C15196-2B81-4950-BB99-B416C4A02B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Functionality</t>
   </si>
@@ -69,12 +69,6 @@
     <t>Product Preview</t>
   </si>
   <si>
-    <t>Admin Ban user by username</t>
-  </si>
-  <si>
-    <t>Admin Add Product Category</t>
-  </si>
-  <si>
     <t>See categories and filter by them</t>
   </si>
   <si>
@@ -103,6 +97,9 @@
   </si>
   <si>
     <t>Update Product</t>
+  </si>
+  <si>
+    <t>Admin Ban user when on profile</t>
   </si>
 </sst>
 </file>
@@ -125,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +138,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -172,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -180,6 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +517,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -560,7 +564,7 @@
       <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -585,7 +589,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3"/>
     </row>
@@ -594,16 +598,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3"/>
     </row>
@@ -612,7 +616,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="3"/>
     </row>
@@ -621,34 +625,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C20" s="3"/>
     </row>
@@ -657,9 +661,9 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22">
@@ -668,34 +672,25 @@
       <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
basically finished with product page
</commit_message>
<xml_diff>
--- a/files/documentation/Frontend Functionalities.xlsx
+++ b/files/documentation/Frontend Functionalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C15196-2B81-4950-BB99-B416C4A02B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD928DC-400D-407E-949F-DCD84651840E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +573,7 @@
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">

</xml_diff>

<commit_message>
Finished Delete Product Functionality
</commit_message>
<xml_diff>
--- a/files/documentation/Frontend Functionalities.xlsx
+++ b/files/documentation/Frontend Functionalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD928DC-400D-407E-949F-DCD84651840E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B4F66D-1FBF-4537-B0FC-7E90C1A9E85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,7 +645,7 @@
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">

</xml_diff>

<commit_message>
finished delete product by admin + other refactors
</commit_message>
<xml_diff>
--- a/files/documentation/Frontend Functionalities.xlsx
+++ b/files/documentation/Frontend Functionalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B4F66D-1FBF-4537-B0FC-7E90C1A9E85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E0A109-BA45-4705-963F-59890FA4738B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,7 +654,7 @@
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21">
@@ -690,7 +690,7 @@
       <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished ban user / remove user ban
</commit_message>
<xml_diff>
--- a/files/documentation/Frontend Functionalities.xlsx
+++ b/files/documentation/Frontend Functionalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E0A109-BA45-4705-963F-59890FA4738B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB45B6D-8EDB-4904-A61A-E523906F7982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Functionality</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Admin Ban user when on profile</t>
+  </si>
+  <si>
+    <t>Admin Remove Ban</t>
   </si>
 </sst>
 </file>
@@ -464,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,32 +594,32 @@
       <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="3"/>
     </row>
@@ -625,25 +628,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="2"/>
     </row>
@@ -652,7 +655,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -661,7 +664,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -670,27 +673,36 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished search, pagination, recommended products, my products, favorite products
</commit_message>
<xml_diff>
--- a/files/documentation/Frontend Functionalities.xlsx
+++ b/files/documentation/Frontend Functionalities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB45B6D-8EDB-4904-A61A-E523906F7982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0E96E3-1904-4A74-8078-0F1C09CDF0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,7 +585,7 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -621,7 +621,7 @@
       <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
@@ -630,7 +630,7 @@
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18">
@@ -639,7 +639,7 @@
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">

</xml_diff>